<commit_message>
İmam.Hat. unvanı İmam-Hat. olarak değiştirildi.
</commit_message>
<xml_diff>
--- a/maas_verileri.xlsx
+++ b/maas_verileri.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Uz.İm.Hat</t>
   </si>
   <si>
-    <t xml:space="preserve">İmam.Hat.</t>
+    <t xml:space="preserve">İmam-Hat.</t>
   </si>
   <si>
     <t xml:space="preserve">İmam.Hat.(Ş)</t>
@@ -424,7 +424,7 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P15" activeCellId="0" sqref="P15"/>
     </sheetView>
   </sheetViews>
@@ -889,11 +889,11 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.14"/>
@@ -1423,11 +1423,11 @@
   </sheetPr>
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G45" activeCellId="0" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.98"/>
@@ -2126,10 +2126,10 @@
   </sheetPr>
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D244" activeCellId="0" sqref="D244"/>
+      <selection pane="bottomLeft" activeCell="A107" activeCellId="0" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6799,7 +6799,7 @@
   </sheetPr>
   <dimension ref="A1:O321"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C191" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -6822,7 +6822,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="22.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="23.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.84"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="35" min="16" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="36" style="7" width="11.52"/>
   </cols>

</xml_diff>

<commit_message>
unvan ve oranlar güncellendi.
</commit_message>
<xml_diff>
--- a/maas_verileri.xlsx
+++ b/maas_verileri.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2308" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2315" uniqueCount="86">
   <si>
     <t xml:space="preserve">yil</t>
   </si>
@@ -1430,8 +1430,8 @@
   </sheetPr>
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1872,7 +1872,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="E30" s="1" t="n">
         <v>300</v>
@@ -2142,17 +2142,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F304"/>
+  <dimension ref="A1:F311"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A263" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G279" activeCellId="0" sqref="G279"/>
+      <selection pane="bottomLeft" activeCell="B243" activeCellId="0" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="60.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="60.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.18"/>
@@ -2460,58 +2460,58 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="D22" s="1" t="n">
         <v>100</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>115</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>115</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2519,24 +2519,24 @@
         <v>45</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>100</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D27" s="1" t="n">
         <v>115</v>
@@ -2544,44 +2544,44 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2589,69 +2589,69 @@
         <v>15</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2659,13 +2659,13 @@
         <v>16</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2673,13 +2673,13 @@
         <v>16</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2687,13 +2687,13 @@
         <v>16</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2701,13 +2701,13 @@
         <v>16</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,81 +2715,69 @@
         <v>16</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>134</v>
+        <v>48</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>130</v>
+        <v>48</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>46</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2797,10 +2785,10 @@
         <v>22</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="D45" s="1" t="n">
         <v>66</v>
@@ -2811,13 +2799,13 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D46" s="1" t="n">
         <v>66</v>
@@ -2828,13 +2816,13 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D47" s="1" t="n">
         <v>66</v>
@@ -2845,13 +2833,13 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D48" s="1" t="n">
         <v>66</v>
@@ -2862,13 +2850,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="6" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D49" s="1" t="n">
         <v>66</v>
@@ -2882,10 +2870,10 @@
         <v>19</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="D50" s="1" t="n">
         <v>66</v>
@@ -2899,10 +2887,10 @@
         <v>19</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="D51" s="1" t="n">
         <v>66</v>
@@ -2913,138 +2901,150 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D52" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="E52" s="1" t="n">
-        <v>20</v>
-      </c>
       <c r="F52" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="E53" s="1" t="n">
-        <v>20</v>
-      </c>
       <c r="F53" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>134</v>
+        <v>115</v>
       </c>
       <c r="D54" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="E54" s="1" t="n">
-        <v>15</v>
-      </c>
       <c r="F54" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="D55" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="E55" s="1" t="n">
-        <v>15</v>
-      </c>
       <c r="F55" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>110</v>
+        <v>66</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>110</v>
+        <v>66</v>
+      </c>
+      <c r="E57" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>100</v>
+        <v>66</v>
+      </c>
+      <c r="E58" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>100</v>
+        <v>66</v>
+      </c>
+      <c r="E59" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3052,13 +3052,13 @@
         <v>17</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3066,13 +3066,13 @@
         <v>17</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3080,13 +3080,13 @@
         <v>17</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3094,69 +3094,69 @@
         <v>17</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,10 +3164,10 @@
         <v>18</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D68" s="1" t="n">
         <v>65</v>
@@ -3178,10 +3178,10 @@
         <v>18</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D69" s="1" t="n">
         <v>65</v>
@@ -3192,10 +3192,10 @@
         <v>18</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>65</v>
@@ -3206,10 +3206,10 @@
         <v>18</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>65</v>
@@ -3220,7 +3220,7 @@
         <v>18</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C72" s="1" t="n">
         <v>124</v>
@@ -3234,7 +3234,7 @@
         <v>18</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>124</v>
@@ -3245,70 +3245,58 @@
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B74" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B75" s="1" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B76" s="1" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B77" s="1" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3316,10 +3304,10 @@
         <v>29</v>
       </c>
       <c r="B78" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D78" s="1" t="n">
         <v>70</v>
@@ -3333,10 +3321,10 @@
         <v>29</v>
       </c>
       <c r="B79" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D79" s="1" t="n">
         <v>70</v>
@@ -3350,10 +3338,10 @@
         <v>29</v>
       </c>
       <c r="B80" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D80" s="1" t="n">
         <v>70</v>
@@ -3367,10 +3355,10 @@
         <v>29</v>
       </c>
       <c r="B81" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D81" s="1" t="n">
         <v>70</v>
@@ -3384,7 +3372,7 @@
         <v>29</v>
       </c>
       <c r="B82" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>94</v>
@@ -3401,7 +3389,7 @@
         <v>29</v>
       </c>
       <c r="B83" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>94</v>
@@ -3418,7 +3406,7 @@
         <v>29</v>
       </c>
       <c r="B84" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>94</v>
@@ -3435,7 +3423,7 @@
         <v>29</v>
       </c>
       <c r="B85" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>94</v>
@@ -3449,13 +3437,13 @@
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B86" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D86" s="1" t="n">
         <v>70</v>
@@ -3466,13 +3454,13 @@
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B87" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D87" s="1" t="n">
         <v>70</v>
@@ -3483,13 +3471,13 @@
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B88" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D88" s="1" t="n">
         <v>70</v>
@@ -3500,13 +3488,13 @@
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B89" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D89" s="1" t="n">
         <v>70</v>
@@ -3520,10 +3508,10 @@
         <v>35</v>
       </c>
       <c r="B90" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>70</v>
@@ -3537,10 +3525,10 @@
         <v>35</v>
       </c>
       <c r="B91" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D91" s="1" t="n">
         <v>70</v>
@@ -3554,10 +3542,10 @@
         <v>35</v>
       </c>
       <c r="B92" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D92" s="1" t="n">
         <v>70</v>
@@ -3571,10 +3559,10 @@
         <v>35</v>
       </c>
       <c r="B93" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D93" s="1" t="n">
         <v>70</v>
@@ -3588,7 +3576,7 @@
         <v>35</v>
       </c>
       <c r="B94" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>94</v>
@@ -3605,7 +3593,7 @@
         <v>35</v>
       </c>
       <c r="B95" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>94</v>
@@ -3622,7 +3610,7 @@
         <v>35</v>
       </c>
       <c r="B96" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>94</v>
@@ -3639,7 +3627,7 @@
         <v>35</v>
       </c>
       <c r="B97" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>94</v>
@@ -3653,16 +3641,16 @@
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B98" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>46</v>
@@ -3670,16 +3658,16 @@
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B99" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>46</v>
@@ -3687,16 +3675,16 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B100" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>46</v>
@@ -3704,16 +3692,16 @@
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B101" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>46</v>
@@ -3724,10 +3712,10 @@
         <v>33</v>
       </c>
       <c r="B102" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D102" s="1" t="n">
         <v>65</v>
@@ -3741,10 +3729,10 @@
         <v>33</v>
       </c>
       <c r="B103" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D103" s="1" t="n">
         <v>65</v>
@@ -3758,10 +3746,10 @@
         <v>33</v>
       </c>
       <c r="B104" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C104" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D104" s="1" t="n">
         <v>65</v>
@@ -3775,10 +3763,10 @@
         <v>33</v>
       </c>
       <c r="B105" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D105" s="1" t="n">
         <v>65</v>
@@ -3792,7 +3780,7 @@
         <v>33</v>
       </c>
       <c r="B106" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>94</v>
@@ -3809,7 +3797,7 @@
         <v>33</v>
       </c>
       <c r="B107" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C107" s="1" t="n">
         <v>94</v>
@@ -3826,7 +3814,7 @@
         <v>33</v>
       </c>
       <c r="B108" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C108" s="1" t="n">
         <v>94</v>
@@ -3843,7 +3831,7 @@
         <v>33</v>
       </c>
       <c r="B109" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C109" s="1" t="n">
         <v>94</v>
@@ -3857,70 +3845,70 @@
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B110" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C110" s="1" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B111" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C111" s="1" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B112" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C112" s="1" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B113" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C113" s="1" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F113" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3928,10 +3916,10 @@
         <v>29</v>
       </c>
       <c r="B114" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C114" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D114" s="1" t="n">
         <v>70</v>
@@ -3945,10 +3933,10 @@
         <v>29</v>
       </c>
       <c r="B115" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C115" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D115" s="1" t="n">
         <v>70</v>
@@ -3962,10 +3950,10 @@
         <v>29</v>
       </c>
       <c r="B116" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C116" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D116" s="1" t="n">
         <v>70</v>
@@ -3979,10 +3967,10 @@
         <v>29</v>
       </c>
       <c r="B117" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C117" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D117" s="1" t="n">
         <v>70</v>
@@ -3996,7 +3984,7 @@
         <v>29</v>
       </c>
       <c r="B118" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C118" s="1" t="n">
         <v>92</v>
@@ -4013,10 +4001,10 @@
         <v>29</v>
       </c>
       <c r="B119" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C119" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D119" s="1" t="n">
         <v>70</v>
@@ -4030,10 +4018,10 @@
         <v>29</v>
       </c>
       <c r="B120" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C120" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D120" s="1" t="n">
         <v>70</v>
@@ -4047,10 +4035,10 @@
         <v>29</v>
       </c>
       <c r="B121" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C121" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D121" s="1" t="n">
         <v>70</v>
@@ -4061,13 +4049,13 @@
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B122" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C122" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D122" s="1" t="n">
         <v>70</v>
@@ -4078,13 +4066,13 @@
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B123" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C123" s="1" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D123" s="1" t="n">
         <v>70</v>
@@ -4095,13 +4083,13 @@
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B124" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C124" s="1" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D124" s="1" t="n">
         <v>70</v>
@@ -4112,13 +4100,13 @@
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B125" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C125" s="1" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D125" s="1" t="n">
         <v>70</v>
@@ -4132,10 +4120,10 @@
         <v>35</v>
       </c>
       <c r="B126" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C126" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D126" s="1" t="n">
         <v>70</v>
@@ -4149,10 +4137,10 @@
         <v>35</v>
       </c>
       <c r="B127" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C127" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D127" s="1" t="n">
         <v>70</v>
@@ -4166,10 +4154,10 @@
         <v>35</v>
       </c>
       <c r="B128" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C128" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D128" s="1" t="n">
         <v>70</v>
@@ -4183,10 +4171,10 @@
         <v>35</v>
       </c>
       <c r="B129" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C129" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D129" s="1" t="n">
         <v>70</v>
@@ -4200,7 +4188,7 @@
         <v>35</v>
       </c>
       <c r="B130" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C130" s="1" t="n">
         <v>92</v>
@@ -4217,10 +4205,10 @@
         <v>35</v>
       </c>
       <c r="B131" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C131" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D131" s="1" t="n">
         <v>70</v>
@@ -4234,10 +4222,10 @@
         <v>35</v>
       </c>
       <c r="B132" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C132" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D132" s="1" t="n">
         <v>70</v>
@@ -4251,10 +4239,10 @@
         <v>35</v>
       </c>
       <c r="B133" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C133" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D133" s="1" t="n">
         <v>70</v>
@@ -4265,16 +4253,16 @@
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B134" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C134" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D134" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F134" s="6" t="s">
         <v>47</v>
@@ -4282,16 +4270,16 @@
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B135" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C135" s="1" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D135" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F135" s="6" t="s">
         <v>47</v>
@@ -4299,16 +4287,16 @@
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B136" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C136" s="1" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D136" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F136" s="6" t="s">
         <v>47</v>
@@ -4316,16 +4304,16 @@
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B137" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C137" s="1" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D137" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F137" s="6" t="s">
         <v>47</v>
@@ -4336,10 +4324,10 @@
         <v>33</v>
       </c>
       <c r="B138" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C138" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D138" s="1" t="n">
         <v>65</v>
@@ -4353,10 +4341,10 @@
         <v>33</v>
       </c>
       <c r="B139" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C139" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D139" s="1" t="n">
         <v>65</v>
@@ -4370,10 +4358,10 @@
         <v>33</v>
       </c>
       <c r="B140" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C140" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D140" s="1" t="n">
         <v>65</v>
@@ -4387,10 +4375,10 @@
         <v>33</v>
       </c>
       <c r="B141" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C141" s="1" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D141" s="1" t="n">
         <v>65</v>
@@ -4404,7 +4392,7 @@
         <v>33</v>
       </c>
       <c r="B142" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C142" s="1" t="n">
         <v>92</v>
@@ -4421,10 +4409,10 @@
         <v>33</v>
       </c>
       <c r="B143" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C143" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D143" s="1" t="n">
         <v>65</v>
@@ -4438,10 +4426,10 @@
         <v>33</v>
       </c>
       <c r="B144" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C144" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D144" s="1" t="n">
         <v>65</v>
@@ -4455,10 +4443,10 @@
         <v>33</v>
       </c>
       <c r="B145" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C145" s="1" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D145" s="1" t="n">
         <v>65</v>
@@ -4469,70 +4457,70 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B146" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C146" s="1" t="n">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D146" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B147" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C147" s="1" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D147" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B148" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C148" s="1" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D148" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B149" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C149" s="1" t="n">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D149" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4540,7 +4528,7 @@
         <v>29</v>
       </c>
       <c r="B150" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C150" s="1" t="n">
         <v>89</v>
@@ -4557,7 +4545,7 @@
         <v>29</v>
       </c>
       <c r="B151" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C151" s="1" t="n">
         <v>89</v>
@@ -4574,7 +4562,7 @@
         <v>29</v>
       </c>
       <c r="B152" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C152" s="1" t="n">
         <v>89</v>
@@ -4591,10 +4579,10 @@
         <v>29</v>
       </c>
       <c r="B153" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C153" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D153" s="1" t="n">
         <v>70</v>
@@ -4608,10 +4596,10 @@
         <v>29</v>
       </c>
       <c r="B154" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C154" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D154" s="1" t="n">
         <v>70</v>
@@ -4625,10 +4613,10 @@
         <v>29</v>
       </c>
       <c r="B155" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C155" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D155" s="1" t="n">
         <v>70</v>
@@ -4642,10 +4630,10 @@
         <v>29</v>
       </c>
       <c r="B156" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C156" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D156" s="1" t="n">
         <v>70</v>
@@ -4659,7 +4647,7 @@
         <v>29</v>
       </c>
       <c r="B157" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C157" s="1" t="n">
         <v>88</v>
@@ -4673,13 +4661,13 @@
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B158" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C158" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D158" s="1" t="n">
         <v>70</v>
@@ -4690,13 +4678,13 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B159" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C159" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D159" s="1" t="n">
         <v>70</v>
@@ -4707,13 +4695,13 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B160" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C160" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D160" s="1" t="n">
         <v>70</v>
@@ -4724,13 +4712,13 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B161" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C161" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D161" s="1" t="n">
         <v>70</v>
@@ -4744,7 +4732,7 @@
         <v>35</v>
       </c>
       <c r="B162" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C162" s="1" t="n">
         <v>89</v>
@@ -4761,7 +4749,7 @@
         <v>35</v>
       </c>
       <c r="B163" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C163" s="1" t="n">
         <v>89</v>
@@ -4778,7 +4766,7 @@
         <v>35</v>
       </c>
       <c r="B164" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C164" s="1" t="n">
         <v>89</v>
@@ -4795,10 +4783,10 @@
         <v>35</v>
       </c>
       <c r="B165" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C165" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D165" s="1" t="n">
         <v>70</v>
@@ -4812,10 +4800,10 @@
         <v>35</v>
       </c>
       <c r="B166" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C166" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D166" s="1" t="n">
         <v>70</v>
@@ -4829,10 +4817,10 @@
         <v>35</v>
       </c>
       <c r="B167" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C167" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D167" s="1" t="n">
         <v>70</v>
@@ -4846,10 +4834,10 @@
         <v>35</v>
       </c>
       <c r="B168" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C168" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D168" s="1" t="n">
         <v>70</v>
@@ -4863,7 +4851,7 @@
         <v>35</v>
       </c>
       <c r="B169" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C169" s="1" t="n">
         <v>88</v>
@@ -4877,16 +4865,16 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B170" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C170" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D170" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F170" s="6" t="s">
         <v>48</v>
@@ -4894,16 +4882,16 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B171" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C171" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D171" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F171" s="6" t="s">
         <v>48</v>
@@ -4911,16 +4899,16 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B172" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C172" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D172" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F172" s="6" t="s">
         <v>48</v>
@@ -4928,16 +4916,16 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B173" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C173" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D173" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F173" s="6" t="s">
         <v>48</v>
@@ -4948,7 +4936,7 @@
         <v>33</v>
       </c>
       <c r="B174" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C174" s="1" t="n">
         <v>89</v>
@@ -4965,7 +4953,7 @@
         <v>33</v>
       </c>
       <c r="B175" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C175" s="1" t="n">
         <v>89</v>
@@ -4982,7 +4970,7 @@
         <v>33</v>
       </c>
       <c r="B176" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C176" s="1" t="n">
         <v>89</v>
@@ -4999,10 +4987,10 @@
         <v>33</v>
       </c>
       <c r="B177" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C177" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D177" s="1" t="n">
         <v>65</v>
@@ -5016,10 +5004,10 @@
         <v>33</v>
       </c>
       <c r="B178" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C178" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D178" s="1" t="n">
         <v>65</v>
@@ -5033,10 +5021,10 @@
         <v>33</v>
       </c>
       <c r="B179" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C179" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D179" s="1" t="n">
         <v>65</v>
@@ -5050,10 +5038,10 @@
         <v>33</v>
       </c>
       <c r="B180" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C180" s="1" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D180" s="1" t="n">
         <v>65</v>
@@ -5067,7 +5055,7 @@
         <v>33</v>
       </c>
       <c r="B181" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C181" s="1" t="n">
         <v>88</v>
@@ -5081,82 +5069,70 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B182" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C182" s="1" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D182" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="E182" s="1" t="n">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="F182" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B183" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C183" s="1" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D183" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="E183" s="1" t="n">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="F183" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B184" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C184" s="1" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D184" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="E184" s="1" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="F184" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B185" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C185" s="1" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D185" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="E185" s="1" t="n">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="F185" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5164,16 +5140,16 @@
         <v>28</v>
       </c>
       <c r="B186" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C186" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D186" s="1" t="n">
         <v>70</v>
       </c>
       <c r="E186" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F186" s="6" t="s">
         <v>46</v>
@@ -5184,16 +5160,16 @@
         <v>28</v>
       </c>
       <c r="B187" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C187" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D187" s="1" t="n">
         <v>70</v>
       </c>
       <c r="E187" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F187" s="6" t="s">
         <v>46</v>
@@ -5201,19 +5177,19 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B188" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C188" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D188" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E188" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F188" s="6" t="s">
         <v>46</v>
@@ -5221,19 +5197,19 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B189" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C189" s="1" t="n">
         <v>95</v>
       </c>
       <c r="D189" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E189" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F189" s="6" t="s">
         <v>46</v>
@@ -5241,16 +5217,16 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B190" s="1" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C190" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D190" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E190" s="1" t="n">
         <v>15</v>
@@ -5261,16 +5237,16 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B191" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C191" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D191" s="1" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E191" s="1" t="n">
         <v>15</v>
@@ -5284,16 +5260,16 @@
         <v>32</v>
       </c>
       <c r="B192" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C192" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D192" s="1" t="n">
         <v>65</v>
       </c>
       <c r="E192" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F192" s="6" t="s">
         <v>46</v>
@@ -5304,16 +5280,16 @@
         <v>32</v>
       </c>
       <c r="B193" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C193" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D193" s="1" t="n">
         <v>65</v>
       </c>
       <c r="E193" s="1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F193" s="6" t="s">
         <v>46</v>
@@ -5324,10 +5300,10 @@
         <v>32</v>
       </c>
       <c r="B194" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C194" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D194" s="1" t="n">
         <v>65</v>
@@ -5344,10 +5320,10 @@
         <v>32</v>
       </c>
       <c r="B195" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C195" s="1" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D195" s="1" t="n">
         <v>65</v>
@@ -5361,19 +5337,19 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B196" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C196" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D196" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E196" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F196" s="6" t="s">
         <v>46</v>
@@ -5381,19 +5357,19 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B197" s="1" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C197" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D197" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E197" s="1" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F197" s="6" t="s">
         <v>46</v>
@@ -5401,16 +5377,16 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B198" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C198" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D198" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E198" s="1" t="n">
         <v>15</v>
@@ -5421,16 +5397,16 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B199" s="1" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C199" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D199" s="1" t="n">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E199" s="1" t="n">
         <v>15</v>
@@ -5441,19 +5417,19 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B200" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C200" s="1" t="n">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="D200" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E200" s="1" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F200" s="6" t="s">
         <v>46</v>
@@ -5461,19 +5437,19 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B201" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C201" s="1" t="n">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="D201" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E201" s="1" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F201" s="6" t="s">
         <v>46</v>
@@ -5481,19 +5457,19 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B202" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C202" s="1" t="n">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="D202" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E202" s="1" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F202" s="6" t="s">
         <v>46</v>
@@ -5501,36 +5477,36 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="6" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B203" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C203" s="1" t="n">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="D203" s="1" t="n">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E203" s="1" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F203" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="7" t="s">
-        <v>49</v>
+      <c r="A204" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B204" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C204" s="1" t="n">
-        <v>95</v>
+        <v>140</v>
       </c>
       <c r="D204" s="1" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E204" s="1" t="n">
         <v>40</v>
@@ -5540,17 +5516,17 @@
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="7" t="s">
-        <v>49</v>
+      <c r="A205" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B205" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C205" s="1" t="n">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="D205" s="1" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E205" s="1" t="n">
         <v>40</v>
@@ -5560,17 +5536,17 @@
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="7" t="s">
-        <v>49</v>
+      <c r="A206" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B206" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C206" s="1" t="n">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="D206" s="1" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E206" s="1" t="n">
         <v>30</v>
@@ -5580,17 +5556,17 @@
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="7" t="s">
-        <v>49</v>
+      <c r="A207" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="B207" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C207" s="1" t="n">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="D207" s="1" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E207" s="1" t="n">
         <v>30</v>
@@ -5600,8 +5576,8 @@
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="6" t="s">
-        <v>31</v>
+      <c r="A208" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B208" s="1" t="n">
         <v>1</v>
@@ -5620,8 +5596,8 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="6" t="s">
-        <v>31</v>
+      <c r="A209" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B209" s="1" t="n">
         <v>2</v>
@@ -5640,8 +5616,8 @@
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="6" t="s">
-        <v>31</v>
+      <c r="A210" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B210" s="1" t="n">
         <v>3</v>
@@ -5660,8 +5636,8 @@
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="6" t="s">
-        <v>31</v>
+      <c r="A211" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B211" s="1" t="n">
         <v>4</v>
@@ -5681,58 +5657,82 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B212" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C212" s="1" t="n">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D212" s="1" t="n">
-        <v>110</v>
+        <v>70</v>
+      </c>
+      <c r="E212" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="F212" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B213" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C213" s="1" t="n">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D213" s="1" t="n">
-        <v>110</v>
+        <v>70</v>
+      </c>
+      <c r="E213" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="F213" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B214" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C214" s="1" t="n">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D214" s="1" t="n">
-        <v>100</v>
+        <v>70</v>
+      </c>
+      <c r="E214" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="F214" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="6" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B215" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C215" s="1" t="n">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D215" s="1" t="n">
-        <v>100</v>
+        <v>70</v>
+      </c>
+      <c r="E215" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="F215" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5740,13 +5740,13 @@
         <v>24</v>
       </c>
       <c r="B216" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C216" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D216" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5754,13 +5754,13 @@
         <v>24</v>
       </c>
       <c r="B217" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C217" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D217" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5768,13 +5768,13 @@
         <v>24</v>
       </c>
       <c r="B218" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C218" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D218" s="1" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5782,13 +5782,13 @@
         <v>24</v>
       </c>
       <c r="B219" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C219" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D219" s="1" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5796,13 +5796,13 @@
         <v>24</v>
       </c>
       <c r="B220" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C220" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D220" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5810,13 +5810,13 @@
         <v>24</v>
       </c>
       <c r="B221" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C221" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D221" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5824,13 +5824,13 @@
         <v>24</v>
       </c>
       <c r="B222" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C222" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D222" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5838,7 +5838,7 @@
         <v>24</v>
       </c>
       <c r="B223" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C223" s="1" t="n">
         <v>48</v>
@@ -5849,58 +5849,58 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B224" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C224" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D224" s="1" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B225" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C225" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D225" s="1" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B226" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C226" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D226" s="1" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B227" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C227" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D227" s="1" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5908,13 +5908,13 @@
         <v>25</v>
       </c>
       <c r="B228" s="1" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C228" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D228" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5922,13 +5922,13 @@
         <v>25</v>
       </c>
       <c r="B229" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C229" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D229" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5936,13 +5936,13 @@
         <v>25</v>
       </c>
       <c r="B230" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C230" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D230" s="1" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5950,13 +5950,13 @@
         <v>25</v>
       </c>
       <c r="B231" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C231" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D231" s="1" t="n">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5964,13 +5964,13 @@
         <v>25</v>
       </c>
       <c r="B232" s="1" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C232" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D232" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5978,13 +5978,13 @@
         <v>25</v>
       </c>
       <c r="B233" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C233" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D233" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5992,13 +5992,13 @@
         <v>25</v>
       </c>
       <c r="B234" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C234" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D234" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6006,7 +6006,7 @@
         <v>25</v>
       </c>
       <c r="B235" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C235" s="1" t="n">
         <v>48</v>
@@ -6017,100 +6017,100 @@
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B236" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C236" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D236" s="1" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B237" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C237" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D237" s="1" t="n">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B238" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C238" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D238" s="1" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B239" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C239" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D239" s="1" t="n">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B240" s="1" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C240" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D240" s="1" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B241" s="1" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C241" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D241" s="1" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="6" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B242" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C242" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D242" s="1" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6118,21 +6118,21 @@
         <v>50</v>
       </c>
       <c r="B243" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C243" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D243" s="1" t="n">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B244" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C244" s="1" t="n">
         <v>49</v>
@@ -6143,24 +6143,24 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B245" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C245" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D245" s="1" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B246" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C246" s="1" t="n">
         <v>49</v>
@@ -6171,24 +6171,24 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B247" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C247" s="1" t="n">
         <v>49</v>
       </c>
       <c r="D247" s="1" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B248" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C248" s="1" t="n">
         <v>49</v>
@@ -6199,10 +6199,10 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B249" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C249" s="1" t="n">
         <v>49</v>
@@ -6213,16 +6213,16 @@
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="6" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B250" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C250" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D250" s="1" t="n">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6230,66 +6230,66 @@
         <v>26</v>
       </c>
       <c r="B251" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C251" s="1" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D251" s="1" t="n">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B252" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C252" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D252" s="1" t="n">
-        <v>90</v>
+        <v>110</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B253" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C253" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D253" s="1" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B254" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C254" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D254" s="1" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B255" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C255" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D255" s="1" t="n">
         <v>90</v>
@@ -6297,44 +6297,44 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B256" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C256" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D256" s="1" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B257" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C257" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D257" s="1" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B258" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C258" s="1" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D258" s="1" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6342,13 +6342,13 @@
         <v>37</v>
       </c>
       <c r="B259" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C259" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D259" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6356,13 +6356,13 @@
         <v>37</v>
       </c>
       <c r="B260" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C260" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D260" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6370,13 +6370,13 @@
         <v>37</v>
       </c>
       <c r="B261" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C261" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D261" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6384,13 +6384,13 @@
         <v>37</v>
       </c>
       <c r="B262" s="1" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C262" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D262" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6398,13 +6398,13 @@
         <v>37</v>
       </c>
       <c r="B263" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C263" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D263" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6412,13 +6412,13 @@
         <v>37</v>
       </c>
       <c r="B264" s="1" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C264" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D264" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6426,111 +6426,111 @@
         <v>37</v>
       </c>
       <c r="B265" s="1" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C265" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D265" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B266" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C266" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D266" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B267" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C267" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D267" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B268" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C268" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D268" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B269" s="1" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C269" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D269" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B270" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C270" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D270" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B271" s="1" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C271" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D271" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B272" s="1" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C272" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D272" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6538,13 +6538,13 @@
         <v>38</v>
       </c>
       <c r="B273" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C273" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D273" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6552,13 +6552,13 @@
         <v>38</v>
       </c>
       <c r="B274" s="1" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C274" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D274" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6566,13 +6566,13 @@
         <v>38</v>
       </c>
       <c r="B275" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C275" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D275" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6580,13 +6580,13 @@
         <v>38</v>
       </c>
       <c r="B276" s="1" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C276" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D276" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6594,13 +6594,13 @@
         <v>38</v>
       </c>
       <c r="B277" s="1" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C277" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D277" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6608,13 +6608,13 @@
         <v>38</v>
       </c>
       <c r="B278" s="1" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C278" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D278" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6622,13 +6622,13 @@
         <v>38</v>
       </c>
       <c r="B279" s="1" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C279" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D279" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6636,7 +6636,7 @@
         <v>38</v>
       </c>
       <c r="B280" s="1" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C280" s="1" t="n">
         <v>44</v>
@@ -6647,100 +6647,100 @@
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B281" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C281" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D281" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B282" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C282" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D282" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B283" s="1" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C283" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D283" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B284" s="1" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C284" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D284" s="1" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B285" s="1" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C285" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D285" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B286" s="1" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C286" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D286" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B287" s="1" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C287" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D287" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6748,21 +6748,21 @@
         <v>39</v>
       </c>
       <c r="B288" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C288" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D288" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B289" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C289" s="1" t="n">
         <v>45</v>
@@ -6773,10 +6773,10 @@
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B290" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C290" s="1" t="n">
         <v>45</v>
@@ -6787,10 +6787,10 @@
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B291" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C291" s="1" t="n">
         <v>45</v>
@@ -6801,24 +6801,24 @@
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B292" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C292" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D292" s="1" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B293" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C293" s="1" t="n">
         <v>45</v>
@@ -6829,10 +6829,10 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B294" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C294" s="1" t="n">
         <v>45</v>
@@ -6843,16 +6843,16 @@
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B295" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C295" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D295" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6860,21 +6860,21 @@
         <v>36</v>
       </c>
       <c r="B296" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C296" s="1" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D296" s="1" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B297" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C297" s="1" t="n">
         <v>45</v>
@@ -6885,10 +6885,10 @@
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B298" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C298" s="1" t="n">
         <v>45</v>
@@ -6899,10 +6899,10 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B299" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C299" s="1" t="n">
         <v>45</v>
@@ -6913,24 +6913,24 @@
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B300" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C300" s="1" t="n">
         <v>45</v>
       </c>
       <c r="D300" s="1" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B301" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C301" s="1" t="n">
         <v>45</v>
@@ -6941,10 +6941,10 @@
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B302" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C302" s="1" t="n">
         <v>45</v>
@@ -6955,16 +6955,16 @@
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B303" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C303" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D303" s="1" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6972,12 +6972,110 @@
         <v>40</v>
       </c>
       <c r="B304" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C304" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D304" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A305" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B305" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C305" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D305" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A306" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B306" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C306" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D306" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A307" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B307" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C307" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D307" s="1" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A308" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B308" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C308" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D308" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A309" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B309" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C309" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D309" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A310" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B310" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C310" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D310" s="1" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A311" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B311" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C304" s="1" t="n">
+      <c r="C311" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="D304" s="1" t="n">
+      <c r="D311" s="1" t="n">
         <v>70</v>
       </c>
     </row>
@@ -7000,11 +7098,11 @@
   <dimension ref="A1:O321"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C191" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C236" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A191" activeCellId="0" sqref="A191"/>
-      <selection pane="bottomRight" activeCell="C181" activeCellId="0" sqref="C181"/>
+      <selection pane="bottomLeft" activeCell="A236" activeCellId="0" sqref="A236"/>
+      <selection pane="bottomRight" activeCell="C242" activeCellId="0" sqref="C242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="18.9" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15615,7 +15713,7 @@
         <v>60</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D250" s="1" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
2023 Ocak maaş kat sayıları %16.46 oranında eklendi.
</commit_message>
<xml_diff>
--- a/maas_verileri.xlsx
+++ b/maas_verileri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="aylik_gosterge_puanlari" sheetId="1" state="visible" r:id="rId2"/>
@@ -440,7 +440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -905,14 +905,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1428,7 +1430,18 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
+      <c r="A37" s="5" t="n">
+        <v>44927</v>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>0.388581</v>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>0.123232</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>6.082041</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1442,7 +1455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2170,13 +2183,13 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A424" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="G397" activeCellId="0" sqref="G397"/>
@@ -9069,7 +9082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>

</xml_diff>

<commit_message>
Temmuz 2023 katsayıları eklendi.
</commit_message>
<xml_diff>
--- a/maas_verileri.xlsx
+++ b/maas_verileri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="aylik_gosterge_puanlari" sheetId="1" state="visible" r:id="rId2"/>
@@ -931,12 +931,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1477,6 +1477,20 @@
       </c>
       <c r="D38" s="2" t="n">
         <v>6.787992</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>45122</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>0.509796</v>
+      </c>
+      <c r="C39" s="2" t="n">
+        <v>0.161673</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>7.979285</v>
       </c>
     </row>
   </sheetData>
@@ -2328,7 +2342,7 @@
   </sheetPr>
   <dimension ref="A1:H501"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="I62" activeCellId="0" sqref="I62"/>

</xml_diff>

<commit_message>
2024 Maaş Katsayıları ile diğer maaş verileri işlendi.
</commit_message>
<xml_diff>
--- a/maas_verileri.xlsx
+++ b/maas_verileri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="aylik_gosterge_puanlari" sheetId="1" state="visible" r:id="rId3"/>
@@ -453,7 +453,7 @@
   </sheetPr>
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
@@ -2345,10 +2345,10 @@
   </sheetPr>
   <dimension ref="A1:H503"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C264" activeCellId="0" sqref="C264"/>
+      <selection pane="bottomLeft" activeCell="I119" activeCellId="0" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2549,7 +2549,7 @@
         <v>135</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,7 +2563,7 @@
         <v>135</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2577,7 +2577,7 @@
         <v>135</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2591,7 +2591,7 @@
         <v>135</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,7 +2605,7 @@
         <v>130</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2619,7 +2619,7 @@
         <v>130</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2633,7 +2633,7 @@
         <v>130</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2647,7 +2647,7 @@
         <v>130</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2661,7 +2661,7 @@
         <v>130</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2675,7 +2675,7 @@
         <v>160</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2689,7 +2689,7 @@
         <v>160</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2703,7 +2703,7 @@
         <v>160</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,7 +2717,7 @@
         <v>160</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2731,7 +2731,7 @@
         <v>152</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2745,7 +2745,7 @@
         <v>152</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2759,7 +2759,7 @@
         <v>152</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2773,7 +2773,7 @@
         <v>152</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3827,7 +3827,7 @@
         <v>100</v>
       </c>
       <c r="D97" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>55</v>
@@ -3844,7 +3844,7 @@
         <v>100</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F98" s="7" t="s">
         <v>55</v>
@@ -3861,7 +3861,7 @@
         <v>100</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F99" s="7" t="s">
         <v>55</v>
@@ -3878,7 +3878,7 @@
         <v>100</v>
       </c>
       <c r="D100" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F100" s="7" t="s">
         <v>55</v>
@@ -3895,7 +3895,7 @@
         <v>93</v>
       </c>
       <c r="D101" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F101" s="7" t="s">
         <v>55</v>
@@ -3912,7 +3912,7 @@
         <v>93</v>
       </c>
       <c r="D102" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F102" s="7" t="s">
         <v>55</v>
@@ -3929,7 +3929,7 @@
         <v>93</v>
       </c>
       <c r="D103" s="1" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F103" s="7" t="s">
         <v>55</v>
@@ -3946,7 +3946,7 @@
         <v>93</v>
       </c>
       <c r="D104" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F104" s="7" t="s">
         <v>55</v>
@@ -3963,7 +3963,7 @@
         <v>93</v>
       </c>
       <c r="D105" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F105" s="7" t="s">
         <v>55</v>
@@ -3980,7 +3980,7 @@
         <v>93</v>
       </c>
       <c r="D106" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F106" s="7" t="s">
         <v>55</v>
@@ -3997,7 +3997,7 @@
         <v>64</v>
       </c>
       <c r="D107" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F107" s="7" t="s">
         <v>56</v>
@@ -4014,7 +4014,7 @@
         <v>64</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F108" s="7" t="s">
         <v>56</v>
@@ -4031,7 +4031,7 @@
         <v>64</v>
       </c>
       <c r="D109" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F109" s="7" t="s">
         <v>56</v>
@@ -4048,7 +4048,7 @@
         <v>64</v>
       </c>
       <c r="D110" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F110" s="7" t="s">
         <v>56</v>
@@ -4065,7 +4065,7 @@
         <v>64</v>
       </c>
       <c r="D111" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F111" s="7" t="s">
         <v>56</v>
@@ -4082,7 +4082,7 @@
         <v>61</v>
       </c>
       <c r="D112" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>56</v>
@@ -4099,7 +4099,7 @@
         <v>61</v>
       </c>
       <c r="D113" s="1" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>56</v>
@@ -4116,7 +4116,7 @@
         <v>61</v>
       </c>
       <c r="D114" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>56</v>
@@ -4133,7 +4133,7 @@
         <v>61</v>
       </c>
       <c r="D115" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F115" s="7" t="s">
         <v>56</v>
@@ -4150,7 +4150,7 @@
         <v>61</v>
       </c>
       <c r="D116" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F116" s="7" t="s">
         <v>56</v>
@@ -4167,7 +4167,7 @@
         <v>100</v>
       </c>
       <c r="D117" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F117" s="7" t="s">
         <v>55</v>
@@ -4184,7 +4184,7 @@
         <v>100</v>
       </c>
       <c r="D118" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F118" s="7" t="s">
         <v>55</v>
@@ -4201,7 +4201,7 @@
         <v>100</v>
       </c>
       <c r="D119" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F119" s="7" t="s">
         <v>55</v>
@@ -4218,7 +4218,7 @@
         <v>100</v>
       </c>
       <c r="D120" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F120" s="7" t="s">
         <v>55</v>
@@ -4235,7 +4235,7 @@
         <v>93</v>
       </c>
       <c r="D121" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>55</v>
@@ -4252,7 +4252,7 @@
         <v>93</v>
       </c>
       <c r="D122" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F122" s="7" t="s">
         <v>55</v>
@@ -4269,7 +4269,7 @@
         <v>93</v>
       </c>
       <c r="D123" s="1" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F123" s="7" t="s">
         <v>55</v>
@@ -4286,7 +4286,7 @@
         <v>93</v>
       </c>
       <c r="D124" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F124" s="7" t="s">
         <v>55</v>
@@ -4303,7 +4303,7 @@
         <v>93</v>
       </c>
       <c r="D125" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F125" s="7" t="s">
         <v>55</v>
@@ -4320,7 +4320,7 @@
         <v>93</v>
       </c>
       <c r="D126" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F126" s="7" t="s">
         <v>55</v>
@@ -4337,7 +4337,7 @@
         <v>64</v>
       </c>
       <c r="D127" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F127" s="7" t="s">
         <v>56</v>
@@ -4354,7 +4354,7 @@
         <v>64</v>
       </c>
       <c r="D128" s="1" t="n">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F128" s="7" t="s">
         <v>56</v>
@@ -4371,7 +4371,7 @@
         <v>64</v>
       </c>
       <c r="D129" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F129" s="7" t="s">
         <v>56</v>
@@ -4388,7 +4388,7 @@
         <v>64</v>
       </c>
       <c r="D130" s="1" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F130" s="7" t="s">
         <v>56</v>
@@ -4405,7 +4405,7 @@
         <v>64</v>
       </c>
       <c r="D131" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F131" s="7" t="s">
         <v>56</v>
@@ -4422,7 +4422,7 @@
         <v>61</v>
       </c>
       <c r="D132" s="1" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F132" s="7" t="s">
         <v>56</v>
@@ -4439,7 +4439,7 @@
         <v>61</v>
       </c>
       <c r="D133" s="1" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="F133" s="7" t="s">
         <v>56</v>
@@ -4456,7 +4456,7 @@
         <v>61</v>
       </c>
       <c r="D134" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F134" s="7" t="s">
         <v>56</v>
@@ -4473,7 +4473,7 @@
         <v>61</v>
       </c>
       <c r="D135" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F135" s="7" t="s">
         <v>56</v>
@@ -4490,7 +4490,7 @@
         <v>61</v>
       </c>
       <c r="D136" s="1" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F136" s="7" t="s">
         <v>56</v>
@@ -4504,7 +4504,7 @@
         <v>1</v>
       </c>
       <c r="C137" s="1" t="n">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D137" s="1" t="n">
         <v>65</v>
@@ -4521,7 +4521,7 @@
         <v>2</v>
       </c>
       <c r="C138" s="1" t="n">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D138" s="1" t="n">
         <v>65</v>
@@ -4538,7 +4538,7 @@
         <v>3</v>
       </c>
       <c r="C139" s="1" t="n">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D139" s="1" t="n">
         <v>65</v>
@@ -4555,7 +4555,7 @@
         <v>4</v>
       </c>
       <c r="C140" s="1" t="n">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="D140" s="1" t="n">
         <v>65</v>
@@ -4572,7 +4572,7 @@
         <v>5</v>
       </c>
       <c r="C141" s="1" t="n">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D141" s="1" t="n">
         <v>65</v>
@@ -4589,7 +4589,7 @@
         <v>6</v>
       </c>
       <c r="C142" s="1" t="n">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D142" s="1" t="n">
         <v>65</v>
@@ -4606,7 +4606,7 @@
         <v>7</v>
       </c>
       <c r="C143" s="1" t="n">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="D143" s="1" t="n">
         <v>65</v>
@@ -4623,7 +4623,7 @@
         <v>8</v>
       </c>
       <c r="C144" s="1" t="n">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D144" s="1" t="n">
         <v>65</v>
@@ -4640,7 +4640,7 @@
         <v>9</v>
       </c>
       <c r="C145" s="1" t="n">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D145" s="1" t="n">
         <v>65</v>
@@ -4657,7 +4657,7 @@
         <v>10</v>
       </c>
       <c r="C146" s="1" t="n">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D146" s="1" t="n">
         <v>65</v>
@@ -4674,7 +4674,7 @@
         <v>1</v>
       </c>
       <c r="C147" s="1" t="n">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="D147" s="1" t="n">
         <v>65</v>
@@ -4691,7 +4691,7 @@
         <v>2</v>
       </c>
       <c r="C148" s="1" t="n">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="D148" s="1" t="n">
         <v>65</v>
@@ -4708,7 +4708,7 @@
         <v>3</v>
       </c>
       <c r="C149" s="1" t="n">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="D149" s="1" t="n">
         <v>65</v>
@@ -4725,7 +4725,7 @@
         <v>4</v>
       </c>
       <c r="C150" s="1" t="n">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="D150" s="1" t="n">
         <v>65</v>
@@ -4742,7 +4742,7 @@
         <v>5</v>
       </c>
       <c r="C151" s="1" t="n">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D151" s="1" t="n">
         <v>65</v>
@@ -4759,7 +4759,7 @@
         <v>6</v>
       </c>
       <c r="C152" s="1" t="n">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D152" s="1" t="n">
         <v>65</v>
@@ -4776,7 +4776,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="1" t="n">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D153" s="1" t="n">
         <v>65</v>
@@ -4793,7 +4793,7 @@
         <v>8</v>
       </c>
       <c r="C154" s="1" t="n">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D154" s="1" t="n">
         <v>65</v>
@@ -4810,7 +4810,7 @@
         <v>9</v>
       </c>
       <c r="C155" s="1" t="n">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D155" s="1" t="n">
         <v>65</v>
@@ -4827,7 +4827,7 @@
         <v>10</v>
       </c>
       <c r="C156" s="1" t="n">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="D156" s="1" t="n">
         <v>65</v>

</xml_diff>

<commit_message>
Baş Vaiz ünvanı Başvaiz olarak güncellendi.
</commit_message>
<xml_diff>
--- a/maas_verileri.xlsx
+++ b/maas_verileri.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="aylik_gosterge_puanlari" sheetId="1" state="visible" r:id="rId3"/>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Uzman Vaiz</t>
   </si>
   <si>
-    <t xml:space="preserve">Baş Vaiz</t>
+    <t xml:space="preserve">Başvaiz</t>
   </si>
   <si>
     <t xml:space="preserve">Cezv.Vaizi</t>
@@ -1512,10 +1512,10 @@
   </sheetPr>
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2345,10 +2345,10 @@
   </sheetPr>
   <dimension ref="A1:H504"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F64" activeCellId="0" sqref="F64"/>
+      <selection pane="bottomLeft" activeCell="H88" activeCellId="0" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
@yahyayildirim gitlab üzerinde yapılan değişiklikler aktarıldı.
</commit_message>
<xml_diff>
--- a/maas_verileri.xlsx
+++ b/maas_verileri.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="aylik_gosterge_puanlari" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="maas_kat_sayilari" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="yan_odeme_puanlari" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="ozel_hizmet_tazminati" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="aylik_gosterge_puanlari" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="maas_kat_sayilari" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="yan_odeme_puanlari" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="ozel_hizmet_tazminati" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="59">
   <si>
     <t xml:space="preserve">yil</t>
   </si>
@@ -118,6 +118,9 @@
     <t xml:space="preserve">Din Hz.Uzm</t>
   </si>
   <si>
+    <t xml:space="preserve">Eğt.Uzmanı</t>
+  </si>
+  <si>
     <t xml:space="preserve">Memur</t>
   </si>
   <si>
@@ -187,9 +190,6 @@
     <t xml:space="preserve">ogrenim</t>
   </si>
   <si>
-    <t xml:space="preserve">Eğitim Uzmanı</t>
-  </si>
-  <si>
     <t xml:space="preserve">Yüksek Okul</t>
   </si>
   <si>
@@ -211,7 +211,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -238,6 +238,13 @@
       <sz val="12"/>
       <name val="Times New Roman Tur"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -283,7 +290,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,6 +335,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,112 +349,6 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,12 +823,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="bottomLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1492,6 +1397,20 @@
       </c>
       <c r="D40" s="2" t="n">
         <v>11.909083</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>45474</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>0.907796</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>0.287892</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>14.208727</v>
       </c>
     </row>
   </sheetData>
@@ -1510,12 +1429,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="bottomLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2073,100 +1992,127 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E41" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E42" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>500</v>
+        <v>600</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <v>300</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>1</v>
@@ -2177,7 +2123,7 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>1</v>
@@ -2188,7 +2134,7 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>1</v>
@@ -2199,7 +2145,7 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>1</v>
@@ -2207,13 +2153,10 @@
       <c r="C50" s="1" t="n">
         <v>500</v>
       </c>
-      <c r="D50" s="1" t="n">
-        <v>175</v>
-      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>1</v>
@@ -2224,7 +2167,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>1</v>
@@ -2235,7 +2178,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>1</v>
@@ -2246,7 +2189,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>1</v>
@@ -2257,7 +2200,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>1</v>
@@ -2268,64 +2211,166 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>500</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B63" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="6" t="n">
+      <c r="B64" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C56" s="6" t="n">
+      <c r="C64" s="1" t="n">
         <v>500</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C65" s="6" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2346,9 +2391,9 @@
   <dimension ref="A1:H504"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H88" activeCellId="0" sqref="H88"/>
+      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2371,16 +2416,16 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2986,9 +3031,9 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>54</v>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>1</v>
@@ -3000,9 +3045,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
-        <v>54</v>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>2</v>
@@ -3014,9 +3059,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>54</v>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>3</v>
@@ -3028,9 +3073,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
-        <v>54</v>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>4</v>
@@ -3042,9 +3087,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
-        <v>54</v>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="11" t="s">
+        <v>31</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>5</v>
@@ -4852,7 +4897,7 @@
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B158" s="1" t="n">
         <v>1</v>
@@ -4872,7 +4917,7 @@
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B159" s="1" t="n">
         <v>2</v>
@@ -4892,7 +4937,7 @@
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B160" s="1" t="n">
         <v>3</v>
@@ -4912,7 +4957,7 @@
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B161" s="1" t="n">
         <v>4</v>
@@ -4932,7 +4977,7 @@
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B162" s="1" t="n">
         <v>1</v>
@@ -4952,7 +4997,7 @@
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B163" s="1" t="n">
         <v>2</v>
@@ -4972,7 +5017,7 @@
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B164" s="1" t="n">
         <v>3</v>
@@ -4992,7 +5037,7 @@
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B165" s="1" t="n">
         <v>4</v>
@@ -5012,7 +5057,7 @@
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B166" s="1" t="n">
         <v>5</v>
@@ -5032,7 +5077,7 @@
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B167" s="1" t="n">
         <v>6</v>
@@ -5052,7 +5097,7 @@
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B168" s="1" t="n">
         <v>1</v>
@@ -5069,7 +5114,7 @@
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B169" s="1" t="n">
         <v>2</v>
@@ -5086,7 +5131,7 @@
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B170" s="1" t="n">
         <v>3</v>
@@ -5103,7 +5148,7 @@
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B171" s="1" t="n">
         <v>4</v>
@@ -5120,7 +5165,7 @@
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B172" s="1" t="n">
         <v>5</v>
@@ -5137,7 +5182,7 @@
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B173" s="1" t="n">
         <v>6</v>
@@ -5154,7 +5199,7 @@
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B174" s="1" t="n">
         <v>7</v>
@@ -5171,7 +5216,7 @@
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B175" s="1" t="n">
         <v>8</v>
@@ -5188,7 +5233,7 @@
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B176" s="1" t="n">
         <v>9</v>
@@ -5205,7 +5250,7 @@
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B177" s="1" t="n">
         <v>10</v>
@@ -5222,7 +5267,7 @@
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B178" s="1" t="n">
         <v>11</v>
@@ -5239,7 +5284,7 @@
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B179" s="1" t="n">
         <v>12</v>
@@ -5256,7 +5301,7 @@
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B180" s="1" t="n">
         <v>13</v>
@@ -5273,7 +5318,7 @@
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B181" s="1" t="n">
         <v>14</v>
@@ -5290,7 +5335,7 @@
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B182" s="1" t="n">
         <v>15</v>
@@ -5307,7 +5352,7 @@
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B183" s="1" t="n">
         <v>1</v>
@@ -5324,7 +5369,7 @@
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B184" s="1" t="n">
         <v>2</v>
@@ -5341,7 +5386,7 @@
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B185" s="1" t="n">
         <v>3</v>
@@ -5358,7 +5403,7 @@
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B186" s="1" t="n">
         <v>4</v>
@@ -5375,7 +5420,7 @@
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B187" s="1" t="n">
         <v>5</v>
@@ -5392,7 +5437,7 @@
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B188" s="1" t="n">
         <v>6</v>
@@ -5409,7 +5454,7 @@
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B189" s="1" t="n">
         <v>7</v>
@@ -5426,7 +5471,7 @@
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B190" s="1" t="n">
         <v>8</v>
@@ -5443,7 +5488,7 @@
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B191" s="1" t="n">
         <v>9</v>
@@ -5460,7 +5505,7 @@
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B192" s="1" t="n">
         <v>10</v>
@@ -5477,7 +5522,7 @@
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B193" s="1" t="n">
         <v>11</v>
@@ -5494,7 +5539,7 @@
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B194" s="1" t="n">
         <v>12</v>
@@ -5511,7 +5556,7 @@
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B195" s="1" t="n">
         <v>13</v>
@@ -5528,7 +5573,7 @@
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B196" s="1" t="n">
         <v>14</v>
@@ -5545,7 +5590,7 @@
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B197" s="1" t="n">
         <v>15</v>
@@ -5562,7 +5607,7 @@
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B198" s="1" t="n">
         <v>1</v>
@@ -5579,7 +5624,7 @@
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B199" s="1" t="n">
         <v>2</v>
@@ -5596,7 +5641,7 @@
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B200" s="1" t="n">
         <v>3</v>
@@ -5613,7 +5658,7 @@
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B201" s="1" t="n">
         <v>4</v>
@@ -5630,7 +5675,7 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B202" s="1" t="n">
         <v>5</v>
@@ -5647,7 +5692,7 @@
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B203" s="1" t="n">
         <v>6</v>
@@ -5664,7 +5709,7 @@
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B204" s="1" t="n">
         <v>7</v>
@@ -5681,7 +5726,7 @@
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B205" s="1" t="n">
         <v>8</v>
@@ -5698,7 +5743,7 @@
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B206" s="1" t="n">
         <v>9</v>
@@ -5715,7 +5760,7 @@
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B207" s="1" t="n">
         <v>10</v>
@@ -5732,7 +5777,7 @@
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B208" s="1" t="n">
         <v>11</v>
@@ -5749,7 +5794,7 @@
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B209" s="1" t="n">
         <v>12</v>
@@ -5766,7 +5811,7 @@
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B210" s="1" t="n">
         <v>13</v>
@@ -5783,7 +5828,7 @@
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B211" s="1" t="n">
         <v>14</v>
@@ -5800,7 +5845,7 @@
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B212" s="1" t="n">
         <v>15</v>
@@ -5817,7 +5862,7 @@
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B213" s="1" t="n">
         <v>1</v>
@@ -5837,7 +5882,7 @@
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B214" s="1" t="n">
         <v>2</v>
@@ -5857,7 +5902,7 @@
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B215" s="1" t="n">
         <v>3</v>
@@ -5877,7 +5922,7 @@
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B216" s="1" t="n">
         <v>4</v>
@@ -5897,7 +5942,7 @@
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B217" s="1" t="n">
         <v>1</v>
@@ -5914,7 +5959,7 @@
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B218" s="1" t="n">
         <v>2</v>
@@ -5931,7 +5976,7 @@
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B219" s="1" t="n">
         <v>3</v>
@@ -5948,7 +5993,7 @@
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B220" s="1" t="n">
         <v>4</v>
@@ -5965,7 +6010,7 @@
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B221" s="1" t="n">
         <v>5</v>
@@ -5982,7 +6027,7 @@
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B222" s="1" t="n">
         <v>6</v>
@@ -5999,7 +6044,7 @@
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B223" s="1" t="n">
         <v>7</v>
@@ -6016,7 +6061,7 @@
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B224" s="1" t="n">
         <v>8</v>
@@ -6033,7 +6078,7 @@
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B225" s="1" t="n">
         <v>9</v>
@@ -6050,7 +6095,7 @@
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B226" s="1" t="n">
         <v>10</v>
@@ -6067,7 +6112,7 @@
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B227" s="1" t="n">
         <v>11</v>
@@ -6084,7 +6129,7 @@
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B228" s="1" t="n">
         <v>12</v>
@@ -6101,7 +6146,7 @@
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B229" s="1" t="n">
         <v>13</v>
@@ -6118,7 +6163,7 @@
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B230" s="1" t="n">
         <v>14</v>
@@ -6135,7 +6180,7 @@
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B231" s="1" t="n">
         <v>15</v>
@@ -6152,7 +6197,7 @@
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B232" s="1" t="n">
         <v>1</v>
@@ -6169,7 +6214,7 @@
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B233" s="1" t="n">
         <v>2</v>
@@ -6186,7 +6231,7 @@
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B234" s="1" t="n">
         <v>3</v>
@@ -6203,7 +6248,7 @@
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B235" s="1" t="n">
         <v>4</v>
@@ -6220,7 +6265,7 @@
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B236" s="1" t="n">
         <v>5</v>
@@ -6237,7 +6282,7 @@
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B237" s="1" t="n">
         <v>6</v>
@@ -6254,7 +6299,7 @@
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B238" s="1" t="n">
         <v>7</v>
@@ -6271,7 +6316,7 @@
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B239" s="1" t="n">
         <v>8</v>
@@ -6288,7 +6333,7 @@
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B240" s="1" t="n">
         <v>9</v>
@@ -6305,7 +6350,7 @@
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B241" s="1" t="n">
         <v>10</v>
@@ -6322,7 +6367,7 @@
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B242" s="1" t="n">
         <v>11</v>
@@ -6339,7 +6384,7 @@
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B243" s="1" t="n">
         <v>12</v>
@@ -6356,7 +6401,7 @@
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B244" s="1" t="n">
         <v>13</v>
@@ -6373,7 +6418,7 @@
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B245" s="1" t="n">
         <v>14</v>
@@ -6390,7 +6435,7 @@
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B246" s="1" t="n">
         <v>15</v>
@@ -6407,7 +6452,7 @@
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B247" s="1" t="n">
         <v>1</v>
@@ -6424,7 +6469,7 @@
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B248" s="1" t="n">
         <v>2</v>
@@ -6441,7 +6486,7 @@
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B249" s="1" t="n">
         <v>3</v>
@@ -6458,7 +6503,7 @@
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B250" s="1" t="n">
         <v>4</v>
@@ -6475,7 +6520,7 @@
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B251" s="1" t="n">
         <v>5</v>
@@ -6492,7 +6537,7 @@
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B252" s="1" t="n">
         <v>6</v>
@@ -6509,7 +6554,7 @@
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B253" s="1" t="n">
         <v>7</v>
@@ -6526,7 +6571,7 @@
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B254" s="1" t="n">
         <v>8</v>
@@ -6543,7 +6588,7 @@
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B255" s="1" t="n">
         <v>9</v>
@@ -6560,7 +6605,7 @@
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B256" s="1" t="n">
         <v>10</v>
@@ -6577,7 +6622,7 @@
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B257" s="1" t="n">
         <v>11</v>
@@ -6594,7 +6639,7 @@
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B258" s="1" t="n">
         <v>12</v>
@@ -6611,7 +6656,7 @@
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B259" s="1" t="n">
         <v>13</v>
@@ -6628,7 +6673,7 @@
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B260" s="1" t="n">
         <v>14</v>
@@ -6645,7 +6690,7 @@
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="7" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B261" s="1" t="n">
         <v>15</v>
@@ -6662,7 +6707,7 @@
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B262" s="1" t="n">
         <v>1</v>
@@ -6682,7 +6727,7 @@
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B263" s="1" t="n">
         <v>2</v>
@@ -6702,7 +6747,7 @@
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B264" s="1" t="n">
         <v>3</v>
@@ -6722,7 +6767,7 @@
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B265" s="1" t="n">
         <v>4</v>
@@ -6742,7 +6787,7 @@
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B266" s="1" t="n">
         <v>1</v>
@@ -6762,7 +6807,7 @@
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B267" s="1" t="n">
         <v>2</v>
@@ -6782,7 +6827,7 @@
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B268" s="1" t="n">
         <v>3</v>
@@ -6802,7 +6847,7 @@
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B269" s="1" t="n">
         <v>4</v>
@@ -6822,7 +6867,7 @@
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B270" s="1" t="n">
         <v>5</v>
@@ -6842,7 +6887,7 @@
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B271" s="1" t="n">
         <v>6</v>
@@ -6862,7 +6907,7 @@
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B272" s="1" t="n">
         <v>7</v>
@@ -6882,7 +6927,7 @@
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B273" s="1" t="n">
         <v>8</v>
@@ -6902,7 +6947,7 @@
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B274" s="1" t="n">
         <v>1</v>
@@ -6919,7 +6964,7 @@
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B275" s="1" t="n">
         <v>2</v>
@@ -6936,7 +6981,7 @@
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B276" s="1" t="n">
         <v>3</v>
@@ -6953,7 +6998,7 @@
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B277" s="1" t="n">
         <v>4</v>
@@ -6970,7 +7015,7 @@
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B278" s="1" t="n">
         <v>5</v>
@@ -6987,7 +7032,7 @@
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B279" s="1" t="n">
         <v>6</v>
@@ -7004,7 +7049,7 @@
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B280" s="1" t="n">
         <v>7</v>
@@ -7021,7 +7066,7 @@
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B281" s="1" t="n">
         <v>8</v>
@@ -7038,7 +7083,7 @@
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B282" s="1" t="n">
         <v>9</v>
@@ -7055,7 +7100,7 @@
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B283" s="1" t="n">
         <v>10</v>
@@ -7072,7 +7117,7 @@
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B284" s="1" t="n">
         <v>11</v>
@@ -7089,7 +7134,7 @@
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B285" s="1" t="n">
         <v>12</v>
@@ -7106,7 +7151,7 @@
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B286" s="1" t="n">
         <v>13</v>
@@ -7123,7 +7168,7 @@
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B287" s="1" t="n">
         <v>14</v>
@@ -7140,7 +7185,7 @@
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B288" s="1" t="n">
         <v>15</v>
@@ -7157,7 +7202,7 @@
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B289" s="1" t="n">
         <v>1</v>
@@ -7174,7 +7219,7 @@
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B290" s="1" t="n">
         <v>2</v>
@@ -7191,7 +7236,7 @@
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B291" s="1" t="n">
         <v>3</v>
@@ -7208,7 +7253,7 @@
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B292" s="1" t="n">
         <v>4</v>
@@ -7225,7 +7270,7 @@
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B293" s="1" t="n">
         <v>5</v>
@@ -7242,7 +7287,7 @@
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B294" s="1" t="n">
         <v>6</v>
@@ -7259,7 +7304,7 @@
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B295" s="1" t="n">
         <v>7</v>
@@ -7276,7 +7321,7 @@
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B296" s="1" t="n">
         <v>8</v>
@@ -7293,7 +7338,7 @@
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B297" s="1" t="n">
         <v>9</v>
@@ -7310,7 +7355,7 @@
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B298" s="1" t="n">
         <v>10</v>
@@ -7327,7 +7372,7 @@
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B299" s="1" t="n">
         <v>11</v>
@@ -7344,7 +7389,7 @@
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B300" s="1" t="n">
         <v>12</v>
@@ -7361,7 +7406,7 @@
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B301" s="1" t="n">
         <v>13</v>
@@ -7378,7 +7423,7 @@
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B302" s="1" t="n">
         <v>14</v>
@@ -7395,7 +7440,7 @@
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B303" s="1" t="n">
         <v>15</v>
@@ -7412,7 +7457,7 @@
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B304" s="1" t="n">
         <v>1</v>
@@ -7429,7 +7474,7 @@
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A305" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B305" s="1" t="n">
         <v>2</v>
@@ -7446,7 +7491,7 @@
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A306" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B306" s="1" t="n">
         <v>3</v>
@@ -7463,7 +7508,7 @@
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B307" s="1" t="n">
         <v>4</v>
@@ -7480,7 +7525,7 @@
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A308" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B308" s="1" t="n">
         <v>5</v>
@@ -7497,7 +7542,7 @@
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A309" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B309" s="1" t="n">
         <v>6</v>
@@ -7514,7 +7559,7 @@
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A310" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B310" s="1" t="n">
         <v>7</v>
@@ -7531,7 +7576,7 @@
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A311" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B311" s="1" t="n">
         <v>8</v>
@@ -7548,7 +7593,7 @@
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A312" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B312" s="1" t="n">
         <v>9</v>
@@ -7565,7 +7610,7 @@
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A313" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B313" s="1" t="n">
         <v>10</v>
@@ -7582,7 +7627,7 @@
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A314" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B314" s="1" t="n">
         <v>11</v>
@@ -7599,7 +7644,7 @@
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B315" s="1" t="n">
         <v>12</v>
@@ -7616,7 +7661,7 @@
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A316" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B316" s="1" t="n">
         <v>13</v>
@@ -7633,7 +7678,7 @@
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A317" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B317" s="1" t="n">
         <v>14</v>
@@ -7650,7 +7695,7 @@
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A318" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B318" s="1" t="n">
         <v>15</v>
@@ -7667,7 +7712,7 @@
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A319" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B319" s="1" t="n">
         <v>1</v>
@@ -7681,7 +7726,7 @@
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A320" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B320" s="1" t="n">
         <v>2</v>
@@ -7695,7 +7740,7 @@
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A321" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B321" s="1" t="n">
         <v>3</v>
@@ -7709,7 +7754,7 @@
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A322" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B322" s="1" t="n">
         <v>4</v>
@@ -7723,7 +7768,7 @@
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B323" s="1" t="n">
         <v>5</v>
@@ -7737,7 +7782,7 @@
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A324" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B324" s="1" t="n">
         <v>6</v>
@@ -7751,7 +7796,7 @@
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A325" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B325" s="1" t="n">
         <v>7</v>
@@ -7765,7 +7810,7 @@
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A326" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B326" s="1" t="n">
         <v>8</v>
@@ -7779,7 +7824,7 @@
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A327" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B327" s="1" t="n">
         <v>9</v>
@@ -7793,7 +7838,7 @@
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A328" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B328" s="1" t="n">
         <v>10</v>
@@ -7807,7 +7852,7 @@
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A329" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B329" s="1" t="n">
         <v>11</v>
@@ -7821,7 +7866,7 @@
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A330" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B330" s="1" t="n">
         <v>12</v>
@@ -7835,7 +7880,7 @@
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A331" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B331" s="1" t="n">
         <v>1</v>
@@ -7849,7 +7894,7 @@
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A332" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B332" s="1" t="n">
         <v>2</v>
@@ -7863,7 +7908,7 @@
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A333" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B333" s="1" t="n">
         <v>3</v>
@@ -7877,7 +7922,7 @@
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B334" s="1" t="n">
         <v>4</v>
@@ -7891,7 +7936,7 @@
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A335" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B335" s="1" t="n">
         <v>5</v>
@@ -7905,7 +7950,7 @@
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A336" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B336" s="1" t="n">
         <v>6</v>
@@ -7919,7 +7964,7 @@
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A337" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B337" s="1" t="n">
         <v>7</v>
@@ -7933,7 +7978,7 @@
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A338" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B338" s="1" t="n">
         <v>8</v>
@@ -7947,7 +7992,7 @@
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A339" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B339" s="1" t="n">
         <v>9</v>
@@ -7961,7 +8006,7 @@
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A340" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B340" s="1" t="n">
         <v>10</v>
@@ -7975,7 +8020,7 @@
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A341" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B341" s="1" t="n">
         <v>11</v>
@@ -7989,7 +8034,7 @@
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A342" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B342" s="1" t="n">
         <v>12</v>
@@ -8003,7 +8048,7 @@
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A343" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B343" s="1" t="n">
         <v>13</v>
@@ -8017,7 +8062,7 @@
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A344" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B344" s="1" t="n">
         <v>14</v>
@@ -8031,7 +8076,7 @@
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A345" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B345" s="1" t="n">
         <v>15</v>
@@ -8157,7 +8202,7 @@
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A354" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B354" s="1" t="n">
         <v>1</v>
@@ -8171,7 +8216,7 @@
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A355" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B355" s="1" t="n">
         <v>2</v>
@@ -8185,7 +8230,7 @@
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A356" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B356" s="1" t="n">
         <v>3</v>
@@ -8199,7 +8244,7 @@
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A357" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B357" s="1" t="n">
         <v>4</v>
@@ -8213,7 +8258,7 @@
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A358" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B358" s="1" t="n">
         <v>5</v>
@@ -8227,7 +8272,7 @@
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A359" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B359" s="1" t="n">
         <v>6</v>
@@ -8241,7 +8286,7 @@
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A360" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B360" s="1" t="n">
         <v>7</v>
@@ -8255,7 +8300,7 @@
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A361" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B361" s="1" t="n">
         <v>8</v>
@@ -8269,7 +8314,7 @@
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A362" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B362" s="1" t="n">
         <v>1</v>
@@ -8283,7 +8328,7 @@
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A363" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B363" s="1" t="n">
         <v>2</v>
@@ -8297,7 +8342,7 @@
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A364" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B364" s="1" t="n">
         <v>3</v>
@@ -8311,7 +8356,7 @@
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A365" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B365" s="1" t="n">
         <v>4</v>
@@ -8325,7 +8370,7 @@
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A366" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B366" s="1" t="n">
         <v>5</v>
@@ -8339,7 +8384,7 @@
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A367" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B367" s="1" t="n">
         <v>6</v>
@@ -8353,7 +8398,7 @@
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A368" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B368" s="1" t="n">
         <v>7</v>
@@ -8367,7 +8412,7 @@
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A369" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B369" s="1" t="n">
         <v>8</v>
@@ -8381,7 +8426,7 @@
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A370" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B370" s="1" t="n">
         <v>9</v>
@@ -8395,7 +8440,7 @@
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A371" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B371" s="1" t="n">
         <v>10</v>
@@ -8409,7 +8454,7 @@
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A372" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B372" s="1" t="n">
         <v>11</v>
@@ -8423,7 +8468,7 @@
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A373" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B373" s="1" t="n">
         <v>12</v>
@@ -8437,7 +8482,7 @@
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A374" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B374" s="1" t="n">
         <v>13</v>
@@ -8451,7 +8496,7 @@
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A375" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B375" s="1" t="n">
         <v>14</v>
@@ -8465,7 +8510,7 @@
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A376" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B376" s="1" t="n">
         <v>1</v>
@@ -8479,7 +8524,7 @@
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A377" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B377" s="1" t="n">
         <v>2</v>
@@ -8493,7 +8538,7 @@
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A378" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B378" s="1" t="n">
         <v>3</v>
@@ -8507,7 +8552,7 @@
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A379" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B379" s="1" t="n">
         <v>4</v>
@@ -8521,7 +8566,7 @@
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A380" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B380" s="1" t="n">
         <v>5</v>
@@ -8535,7 +8580,7 @@
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A381" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B381" s="1" t="n">
         <v>6</v>
@@ -8549,7 +8594,7 @@
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A382" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B382" s="1" t="n">
         <v>7</v>
@@ -8563,7 +8608,7 @@
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A383" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B383" s="1" t="n">
         <v>8</v>
@@ -8577,7 +8622,7 @@
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A384" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B384" s="1" t="n">
         <v>9</v>
@@ -8591,7 +8636,7 @@
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A385" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B385" s="1" t="n">
         <v>10</v>
@@ -8605,7 +8650,7 @@
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A386" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B386" s="1" t="n">
         <v>11</v>
@@ -8619,7 +8664,7 @@
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A387" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B387" s="1" t="n">
         <v>12</v>
@@ -8633,7 +8678,7 @@
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A388" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B388" s="1" t="n">
         <v>13</v>
@@ -8647,7 +8692,7 @@
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A389" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B389" s="1" t="n">
         <v>14</v>
@@ -8661,7 +8706,7 @@
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A390" s="7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B390" s="1" t="n">
         <v>15</v>
@@ -8675,7 +8720,7 @@
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A391" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B391" s="1" t="n">
         <v>1</v>
@@ -8689,7 +8734,7 @@
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A392" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B392" s="1" t="n">
         <v>2</v>
@@ -8703,7 +8748,7 @@
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A393" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B393" s="1" t="n">
         <v>3</v>
@@ -8717,7 +8762,7 @@
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A394" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B394" s="1" t="n">
         <v>4</v>
@@ -8731,7 +8776,7 @@
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A395" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B395" s="1" t="n">
         <v>5</v>
@@ -8745,7 +8790,7 @@
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A396" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B396" s="1" t="n">
         <v>6</v>
@@ -8759,7 +8804,7 @@
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A397" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B397" s="1" t="n">
         <v>7</v>
@@ -8773,7 +8818,7 @@
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B398" s="1" t="n">
         <v>8</v>
@@ -8787,7 +8832,7 @@
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B399" s="1" t="n">
         <v>1</v>
@@ -8801,7 +8846,7 @@
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B400" s="1" t="n">
         <v>2</v>
@@ -8815,7 +8860,7 @@
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B401" s="1" t="n">
         <v>3</v>
@@ -8829,7 +8874,7 @@
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B402" s="1" t="n">
         <v>4</v>
@@ -8843,7 +8888,7 @@
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B403" s="1" t="n">
         <v>5</v>
@@ -8857,7 +8902,7 @@
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B404" s="1" t="n">
         <v>6</v>
@@ -8871,7 +8916,7 @@
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B405" s="1" t="n">
         <v>7</v>
@@ -8885,7 +8930,7 @@
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B406" s="1" t="n">
         <v>8</v>
@@ -8899,7 +8944,7 @@
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B407" s="1" t="n">
         <v>1</v>
@@ -8913,7 +8958,7 @@
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B408" s="1" t="n">
         <v>2</v>
@@ -8927,7 +8972,7 @@
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B409" s="1" t="n">
         <v>3</v>
@@ -8941,7 +8986,7 @@
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B410" s="1" t="n">
         <v>4</v>
@@ -8955,7 +9000,7 @@
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B411" s="1" t="n">
         <v>5</v>
@@ -8969,7 +9014,7 @@
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B412" s="1" t="n">
         <v>6</v>
@@ -8983,7 +9028,7 @@
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B413" s="1" t="n">
         <v>7</v>
@@ -8997,7 +9042,7 @@
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B414" s="1" t="n">
         <v>8</v>
@@ -9011,7 +9056,7 @@
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B415" s="1" t="n">
         <v>1</v>
@@ -9025,7 +9070,7 @@
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B416" s="1" t="n">
         <v>2</v>
@@ -9039,7 +9084,7 @@
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B417" s="1" t="n">
         <v>3</v>
@@ -9053,7 +9098,7 @@
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B418" s="1" t="n">
         <v>4</v>
@@ -9067,7 +9112,7 @@
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B419" s="1" t="n">
         <v>5</v>
@@ -9081,7 +9126,7 @@
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B420" s="1" t="n">
         <v>6</v>
@@ -9095,7 +9140,7 @@
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B421" s="1" t="n">
         <v>7</v>
@@ -9109,7 +9154,7 @@
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B422" s="1" t="n">
         <v>8</v>
@@ -9123,7 +9168,7 @@
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B423" s="1" t="n">
         <v>9</v>
@@ -9137,7 +9182,7 @@
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B424" s="1" t="n">
         <v>10</v>
@@ -9151,7 +9196,7 @@
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B425" s="1" t="n">
         <v>11</v>
@@ -9165,7 +9210,7 @@
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B426" s="1" t="n">
         <v>12</v>
@@ -9179,7 +9224,7 @@
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B427" s="1" t="n">
         <v>13</v>
@@ -9193,7 +9238,7 @@
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B428" s="1" t="n">
         <v>14</v>
@@ -9207,7 +9252,7 @@
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B429" s="1" t="n">
         <v>15</v>
@@ -9221,7 +9266,7 @@
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B430" s="1" t="n">
         <v>1</v>
@@ -9235,7 +9280,7 @@
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B431" s="1" t="n">
         <v>2</v>
@@ -9249,7 +9294,7 @@
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B432" s="1" t="n">
         <v>3</v>
@@ -9263,7 +9308,7 @@
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B433" s="1" t="n">
         <v>4</v>
@@ -9277,7 +9322,7 @@
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B434" s="1" t="n">
         <v>5</v>
@@ -9291,7 +9336,7 @@
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B435" s="1" t="n">
         <v>6</v>
@@ -9305,7 +9350,7 @@
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B436" s="1" t="n">
         <v>7</v>
@@ -9319,7 +9364,7 @@
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B437" s="1" t="n">
         <v>8</v>
@@ -9333,7 +9378,7 @@
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B438" s="1" t="n">
         <v>9</v>
@@ -9347,7 +9392,7 @@
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B439" s="1" t="n">
         <v>10</v>
@@ -9361,7 +9406,7 @@
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B440" s="1" t="n">
         <v>11</v>
@@ -9375,7 +9420,7 @@
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B441" s="1" t="n">
         <v>12</v>
@@ -9389,7 +9434,7 @@
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B442" s="1" t="n">
         <v>13</v>
@@ -9403,7 +9448,7 @@
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B443" s="1" t="n">
         <v>14</v>
@@ -9417,7 +9462,7 @@
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B444" s="1" t="n">
         <v>15</v>
@@ -9431,7 +9476,7 @@
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B445" s="1" t="n">
         <v>1</v>
@@ -9445,7 +9490,7 @@
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B446" s="1" t="n">
         <v>2</v>
@@ -9459,7 +9504,7 @@
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B447" s="1" t="n">
         <v>3</v>
@@ -9473,7 +9518,7 @@
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B448" s="1" t="n">
         <v>4</v>
@@ -9487,7 +9532,7 @@
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B449" s="1" t="n">
         <v>5</v>
@@ -9501,7 +9546,7 @@
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B450" s="1" t="n">
         <v>6</v>
@@ -9515,7 +9560,7 @@
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B451" s="1" t="n">
         <v>7</v>
@@ -9529,7 +9574,7 @@
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B452" s="1" t="n">
         <v>8</v>
@@ -9543,7 +9588,7 @@
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B453" s="1" t="n">
         <v>9</v>
@@ -9557,7 +9602,7 @@
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B454" s="1" t="n">
         <v>10</v>
@@ -9571,7 +9616,7 @@
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B455" s="1" t="n">
         <v>11</v>
@@ -9585,7 +9630,7 @@
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B456" s="1" t="n">
         <v>12</v>
@@ -9599,7 +9644,7 @@
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B457" s="1" t="n">
         <v>13</v>
@@ -9613,7 +9658,7 @@
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B458" s="1" t="n">
         <v>14</v>
@@ -9627,7 +9672,7 @@
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B459" s="1" t="n">
         <v>15</v>
@@ -9641,7 +9686,7 @@
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B460" s="1" t="n">
         <v>1</v>
@@ -9655,7 +9700,7 @@
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B461" s="1" t="n">
         <v>2</v>
@@ -9669,7 +9714,7 @@
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B462" s="1" t="n">
         <v>3</v>
@@ -9683,7 +9728,7 @@
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B463" s="1" t="n">
         <v>4</v>
@@ -9697,7 +9742,7 @@
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B464" s="1" t="n">
         <v>5</v>
@@ -9711,7 +9756,7 @@
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B465" s="1" t="n">
         <v>6</v>
@@ -9725,7 +9770,7 @@
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B466" s="1" t="n">
         <v>7</v>
@@ -9739,7 +9784,7 @@
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B467" s="1" t="n">
         <v>8</v>
@@ -9753,7 +9798,7 @@
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B468" s="1" t="n">
         <v>9</v>
@@ -9767,7 +9812,7 @@
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B469" s="1" t="n">
         <v>10</v>
@@ -9781,7 +9826,7 @@
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B470" s="1" t="n">
         <v>11</v>
@@ -9795,7 +9840,7 @@
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B471" s="1" t="n">
         <v>12</v>
@@ -9809,7 +9854,7 @@
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B472" s="1" t="n">
         <v>13</v>
@@ -9823,7 +9868,7 @@
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B473" s="1" t="n">
         <v>14</v>
@@ -9837,7 +9882,7 @@
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A474" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B474" s="1" t="n">
         <v>15</v>
@@ -9851,7 +9896,7 @@
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A475" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B475" s="1" t="n">
         <v>1</v>
@@ -9865,7 +9910,7 @@
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B476" s="1" t="n">
         <v>2</v>
@@ -9879,7 +9924,7 @@
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B477" s="1" t="n">
         <v>3</v>
@@ -9893,7 +9938,7 @@
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A478" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B478" s="1" t="n">
         <v>4</v>
@@ -9907,7 +9952,7 @@
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A479" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B479" s="1" t="n">
         <v>5</v>
@@ -9921,7 +9966,7 @@
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A480" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B480" s="1" t="n">
         <v>6</v>
@@ -9935,7 +9980,7 @@
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B481" s="1" t="n">
         <v>7</v>
@@ -9949,7 +9994,7 @@
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B482" s="1" t="n">
         <v>8</v>
@@ -9963,7 +10008,7 @@
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B483" s="1" t="n">
         <v>9</v>
@@ -9977,7 +10022,7 @@
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B484" s="1" t="n">
         <v>10</v>
@@ -9991,7 +10036,7 @@
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B485" s="1" t="n">
         <v>11</v>
@@ -10005,7 +10050,7 @@
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B486" s="1" t="n">
         <v>12</v>
@@ -10019,7 +10064,7 @@
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B487" s="1" t="n">
         <v>13</v>
@@ -10033,7 +10078,7 @@
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B488" s="1" t="n">
         <v>14</v>
@@ -10047,7 +10092,7 @@
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B489" s="1" t="n">
         <v>15</v>
@@ -10061,7 +10106,7 @@
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B490" s="1" t="n">
         <v>1</v>
@@ -10075,7 +10120,7 @@
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B491" s="1" t="n">
         <v>2</v>
@@ -10089,7 +10134,7 @@
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B492" s="1" t="n">
         <v>3</v>
@@ -10103,7 +10148,7 @@
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B493" s="1" t="n">
         <v>4</v>
@@ -10117,7 +10162,7 @@
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B494" s="1" t="n">
         <v>5</v>
@@ -10131,7 +10176,7 @@
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B495" s="1" t="n">
         <v>6</v>
@@ -10145,7 +10190,7 @@
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B496" s="1" t="n">
         <v>7</v>
@@ -10159,7 +10204,7 @@
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B497" s="1" t="n">
         <v>8</v>
@@ -10173,7 +10218,7 @@
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B498" s="1" t="n">
         <v>9</v>
@@ -10187,7 +10232,7 @@
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B499" s="1" t="n">
         <v>10</v>
@@ -10201,7 +10246,7 @@
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A500" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B500" s="1" t="n">
         <v>11</v>
@@ -10215,7 +10260,7 @@
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A501" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B501" s="1" t="n">
         <v>12</v>
@@ -10229,7 +10274,7 @@
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A502" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B502" s="1" t="n">
         <v>13</v>
@@ -10243,7 +10288,7 @@
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A503" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B503" s="1" t="n">
         <v>14</v>
@@ -10257,7 +10302,7 @@
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A504" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B504" s="1" t="n">
         <v>15</v>

</xml_diff>